<commit_message>
2023 Paper Version 7 Code Update
Many changes and additions, including addition of scatter plots 2020 Jupiter retrievals, better plots of filters for SCT and VLT including the Jovian albedo. MOST IMPORTANTLY I aligned all the computations for k_eff and calibrations with the proper filter shapes specific to SCT and VLT. SCT filters now incorporate the overall system performance, but this is done explicitly in line. I NEED TO CHECK IF IT'S DONE EVERYWHERE NEEDED. ALSO, THERE'S TONS OF HARDCODING OF KEY PARAMETERS AND REARCHITECTNIG IS NEEDED NOT TO HAVE ISSUES ACCIDENTAL ERRORS IF ITEMS NEED UPDATING AND AREN'T UPDATED EVERYWHERE.
</commit_message>
<xml_diff>
--- a/Literature CH4 and NH3 Measurements.xlsx
+++ b/Literature CH4 and NH3 Measurements.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Astronomy\Projects\SAS 2021 Ammonia\Jupiter_NH3_Analysis_P3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA9EAD40-1CC5-46A0-B2E8-581D4D05EF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8659525D-C285-40FA-B939-A17396EA9F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="10980" windowHeight="9810" xr2:uid="{DE140F0E-5E6A-4D54-8374-BA43FF538A80}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DE140F0E-5E6A-4D54-8374-BA43FF538A80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$110</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="42">
   <si>
     <t>Molecule</t>
   </si>
@@ -214,6 +214,27 @@
   </si>
   <si>
     <t>[Owen and Cess, 1975]</t>
+  </si>
+  <si>
+    <t>SPR</t>
+  </si>
+  <si>
+    <t>STB</t>
+  </si>
+  <si>
+    <t>NTB</t>
+  </si>
+  <si>
+    <t>NPR</t>
+  </si>
+  <si>
+    <t>[Moreno et al., 1988]</t>
+  </si>
+  <si>
+    <t>NTrZ</t>
+  </si>
+  <si>
+    <t>[Morena &amp; Molina, 1991]</t>
   </si>
 </sst>
 </file>
@@ -583,24 +604,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52DE5DE2-3EF6-48AC-A4A4-AF66BBBA5C59}">
-  <dimension ref="A1:J74"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:K113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E67" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E74" sqref="E74"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12:F110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.140625" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" customWidth="1"/>
-    <col min="9" max="9" width="29.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" customWidth="1"/>
+    <col min="2" max="2" width="5.26953125" customWidth="1"/>
+    <col min="9" max="9" width="29.26953125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="27.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -632,7 +654,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -665,7 +687,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -695,7 +717,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -725,7 +747,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -758,7 +780,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -788,7 +810,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -818,7 +840,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -851,7 +873,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -881,7 +903,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -911,7 +933,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -924,10 +946,7 @@
       <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="F11" s="1"/>
       <c r="G11">
         <v>24</v>
       </c>
@@ -941,7 +960,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -971,7 +990,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -984,10 +1003,7 @@
       <c r="D13" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="F13" s="1"/>
       <c r="H13">
         <v>1.3</v>
       </c>
@@ -998,7 +1014,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1044,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1059,7 +1075,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1090,7 +1106,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1121,7 +1137,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1152,7 +1168,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1182,7 +1198,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1212,7 +1228,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1242,7 +1258,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -1272,7 +1288,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1302,7 +1318,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -1332,7 +1348,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -1363,7 +1379,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -1394,7 +1410,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -1425,7 +1441,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -1456,7 +1472,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1486,7 +1502,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -1516,7 +1532,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -1546,7 +1562,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -1576,7 +1592,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1606,7 +1622,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -1636,7 +1652,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -1666,7 +1682,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -1696,7 +1712,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -1726,7 +1742,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -1756,7 +1772,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -1786,7 +1802,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>4</v>
       </c>
@@ -1816,7 +1832,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -1846,7 +1862,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -1876,7 +1892,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -1906,7 +1922,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -1936,7 +1952,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -1966,7 +1982,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -1996,7 +2012,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -2026,7 +2042,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>4</v>
       </c>
@@ -2056,7 +2072,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -2086,7 +2102,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -2116,7 +2132,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -2146,7 +2162,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>4</v>
       </c>
@@ -2176,7 +2192,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>4</v>
       </c>
@@ -2206,7 +2222,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>4</v>
       </c>
@@ -2236,7 +2252,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>4</v>
       </c>
@@ -2266,7 +2282,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>4</v>
       </c>
@@ -2296,7 +2312,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>4</v>
       </c>
@@ -2326,7 +2342,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>4</v>
       </c>
@@ -2356,7 +2372,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>4</v>
       </c>
@@ -2386,7 +2402,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>4</v>
       </c>
@@ -2410,7 +2426,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>4</v>
       </c>
@@ -2434,7 +2450,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>4</v>
       </c>
@@ -2458,7 +2474,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>4</v>
       </c>
@@ -2482,7 +2498,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>4</v>
       </c>
@@ -2506,7 +2522,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>4</v>
       </c>
@@ -2530,7 +2546,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>4</v>
       </c>
@@ -2554,7 +2570,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>4</v>
       </c>
@@ -2578,7 +2594,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>4</v>
       </c>
@@ -2602,7 +2618,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>4</v>
       </c>
@@ -2626,7 +2642,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>4</v>
       </c>
@@ -2650,7 +2666,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>4</v>
       </c>
@@ -2674,7 +2690,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>4</v>
       </c>
@@ -2698,7 +2714,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>4</v>
       </c>
@@ -2722,7 +2738,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>4</v>
       </c>
@@ -2746,10 +2762,897 @@
         <v>34</v>
       </c>
     </row>
+    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>4</v>
+      </c>
+      <c r="B75">
+        <v>619</v>
+      </c>
+      <c r="C75" t="s">
+        <v>5</v>
+      </c>
+      <c r="D75" t="s">
+        <v>21</v>
+      </c>
+      <c r="F75">
+        <v>0.97</v>
+      </c>
+      <c r="J75" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>4</v>
+      </c>
+      <c r="B76">
+        <v>619</v>
+      </c>
+      <c r="C76" t="s">
+        <v>5</v>
+      </c>
+      <c r="D76" t="s">
+        <v>21</v>
+      </c>
+      <c r="F76">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="J76" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>4</v>
+      </c>
+      <c r="B77">
+        <v>619</v>
+      </c>
+      <c r="C77" t="s">
+        <v>5</v>
+      </c>
+      <c r="D77" t="s">
+        <v>21</v>
+      </c>
+      <c r="F77">
+        <v>1.62</v>
+      </c>
+      <c r="J77" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>4</v>
+      </c>
+      <c r="B78">
+        <v>619</v>
+      </c>
+      <c r="C78" t="s">
+        <v>5</v>
+      </c>
+      <c r="D78" t="s">
+        <v>21</v>
+      </c>
+      <c r="F78">
+        <v>1.32</v>
+      </c>
+      <c r="J78" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>4</v>
+      </c>
+      <c r="B79">
+        <v>619</v>
+      </c>
+      <c r="C79" t="s">
+        <v>5</v>
+      </c>
+      <c r="D79" t="s">
+        <v>21</v>
+      </c>
+      <c r="F79">
+        <v>0.91</v>
+      </c>
+      <c r="J79" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>4</v>
+      </c>
+      <c r="B80">
+        <v>619</v>
+      </c>
+      <c r="C80" t="s">
+        <v>5</v>
+      </c>
+      <c r="D80" t="s">
+        <v>35</v>
+      </c>
+      <c r="F80">
+        <v>1.76</v>
+      </c>
+      <c r="J80" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>4</v>
+      </c>
+      <c r="B81">
+        <v>619</v>
+      </c>
+      <c r="C81" t="s">
+        <v>5</v>
+      </c>
+      <c r="D81" t="s">
+        <v>36</v>
+      </c>
+      <c r="F81">
+        <v>1.62</v>
+      </c>
+      <c r="J81" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>4</v>
+      </c>
+      <c r="B82">
+        <v>619</v>
+      </c>
+      <c r="C82" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" t="s">
+        <v>25</v>
+      </c>
+      <c r="F82">
+        <v>1.82</v>
+      </c>
+      <c r="J82" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>4</v>
+      </c>
+      <c r="B83">
+        <v>619</v>
+      </c>
+      <c r="C83" t="s">
+        <v>5</v>
+      </c>
+      <c r="D83" t="s">
+        <v>24</v>
+      </c>
+      <c r="F83">
+        <v>2.25</v>
+      </c>
+      <c r="J83" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>4</v>
+      </c>
+      <c r="B84">
+        <v>619</v>
+      </c>
+      <c r="C84" t="s">
+        <v>5</v>
+      </c>
+      <c r="D84" t="s">
+        <v>21</v>
+      </c>
+      <c r="F84">
+        <v>1.85</v>
+      </c>
+      <c r="J84" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>4</v>
+      </c>
+      <c r="B85">
+        <v>619</v>
+      </c>
+      <c r="C85" t="s">
+        <v>5</v>
+      </c>
+      <c r="D85" t="s">
+        <v>23</v>
+      </c>
+      <c r="F85">
+        <v>1.47</v>
+      </c>
+      <c r="J85" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>4</v>
+      </c>
+      <c r="B86">
+        <v>619</v>
+      </c>
+      <c r="C86" t="s">
+        <v>5</v>
+      </c>
+      <c r="D86" t="s">
+        <v>37</v>
+      </c>
+      <c r="F86">
+        <v>1.5</v>
+      </c>
+      <c r="J86" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>4</v>
+      </c>
+      <c r="B87">
+        <v>619</v>
+      </c>
+      <c r="C87" t="s">
+        <v>5</v>
+      </c>
+      <c r="D87" t="s">
+        <v>38</v>
+      </c>
+      <c r="F87">
+        <v>1.95</v>
+      </c>
+      <c r="J87" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>15</v>
+      </c>
+      <c r="B88">
+        <v>647</v>
+      </c>
+      <c r="C88" t="s">
+        <v>5</v>
+      </c>
+      <c r="D88" t="s">
+        <v>21</v>
+      </c>
+      <c r="F88">
+        <v>0.61</v>
+      </c>
+      <c r="J88" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>15</v>
+      </c>
+      <c r="B89">
+        <v>647</v>
+      </c>
+      <c r="C89" t="s">
+        <v>5</v>
+      </c>
+      <c r="D89" t="s">
+        <v>21</v>
+      </c>
+      <c r="F89">
+        <v>0.49</v>
+      </c>
+      <c r="J89" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>15</v>
+      </c>
+      <c r="B90">
+        <v>647</v>
+      </c>
+      <c r="C90" t="s">
+        <v>5</v>
+      </c>
+      <c r="D90" t="s">
+        <v>21</v>
+      </c>
+      <c r="F90">
+        <v>0.77</v>
+      </c>
+      <c r="J90" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>15</v>
+      </c>
+      <c r="B91">
+        <v>647</v>
+      </c>
+      <c r="C91" t="s">
+        <v>5</v>
+      </c>
+      <c r="D91" t="s">
+        <v>21</v>
+      </c>
+      <c r="F91">
+        <v>0.44</v>
+      </c>
+      <c r="J91" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>15</v>
+      </c>
+      <c r="B92">
+        <v>647</v>
+      </c>
+      <c r="C92" t="s">
+        <v>5</v>
+      </c>
+      <c r="D92" t="s">
+        <v>21</v>
+      </c>
+      <c r="F92">
+        <v>0.19</v>
+      </c>
+      <c r="J92" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>15</v>
+      </c>
+      <c r="B93">
+        <v>647</v>
+      </c>
+      <c r="C93" t="s">
+        <v>5</v>
+      </c>
+      <c r="D93" t="s">
+        <v>35</v>
+      </c>
+      <c r="F93">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="J93" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>15</v>
+      </c>
+      <c r="B94">
+        <v>647</v>
+      </c>
+      <c r="C94" t="s">
+        <v>5</v>
+      </c>
+      <c r="D94" t="s">
+        <v>36</v>
+      </c>
+      <c r="F94">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="J94" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>15</v>
+      </c>
+      <c r="B95">
+        <v>647</v>
+      </c>
+      <c r="C95" t="s">
+        <v>5</v>
+      </c>
+      <c r="D95" t="s">
+        <v>25</v>
+      </c>
+      <c r="F95">
+        <v>0.78</v>
+      </c>
+      <c r="J95" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>15</v>
+      </c>
+      <c r="B96">
+        <v>647</v>
+      </c>
+      <c r="C96" t="s">
+        <v>5</v>
+      </c>
+      <c r="D96" t="s">
+        <v>24</v>
+      </c>
+      <c r="F96">
+        <v>0.98</v>
+      </c>
+      <c r="J96" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>15</v>
+      </c>
+      <c r="B97">
+        <v>647</v>
+      </c>
+      <c r="C97" t="s">
+        <v>5</v>
+      </c>
+      <c r="D97" t="s">
+        <v>21</v>
+      </c>
+      <c r="F97">
+        <v>0.78</v>
+      </c>
+      <c r="J97" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>15</v>
+      </c>
+      <c r="B98">
+        <v>647</v>
+      </c>
+      <c r="C98" t="s">
+        <v>5</v>
+      </c>
+      <c r="D98" t="s">
+        <v>23</v>
+      </c>
+      <c r="F98">
+        <v>0.49</v>
+      </c>
+      <c r="J98" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>15</v>
+      </c>
+      <c r="B99">
+        <v>647</v>
+      </c>
+      <c r="C99" t="s">
+        <v>5</v>
+      </c>
+      <c r="D99" t="s">
+        <v>37</v>
+      </c>
+      <c r="F99">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="J99" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>15</v>
+      </c>
+      <c r="B100">
+        <v>647</v>
+      </c>
+      <c r="C100" t="s">
+        <v>5</v>
+      </c>
+      <c r="D100" t="s">
+        <v>38</v>
+      </c>
+      <c r="F100">
+        <v>0.72</v>
+      </c>
+      <c r="J100" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>4</v>
+      </c>
+      <c r="B101">
+        <v>619</v>
+      </c>
+      <c r="C101" t="s">
+        <v>5</v>
+      </c>
+      <c r="D101" t="s">
+        <v>40</v>
+      </c>
+      <c r="F101">
+        <v>1.3</v>
+      </c>
+      <c r="J101" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>4</v>
+      </c>
+      <c r="B102">
+        <v>619</v>
+      </c>
+      <c r="C102" t="s">
+        <v>5</v>
+      </c>
+      <c r="D102" t="s">
+        <v>23</v>
+      </c>
+      <c r="F102">
+        <v>1.57</v>
+      </c>
+      <c r="J102" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>4</v>
+      </c>
+      <c r="B103">
+        <v>619</v>
+      </c>
+      <c r="C103" t="s">
+        <v>5</v>
+      </c>
+      <c r="D103" t="s">
+        <v>21</v>
+      </c>
+      <c r="F103">
+        <v>1.44</v>
+      </c>
+      <c r="J103" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>4</v>
+      </c>
+      <c r="B104">
+        <v>619</v>
+      </c>
+      <c r="C104" t="s">
+        <v>5</v>
+      </c>
+      <c r="D104" t="s">
+        <v>24</v>
+      </c>
+      <c r="F104">
+        <v>1.57</v>
+      </c>
+      <c r="J104" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>4</v>
+      </c>
+      <c r="B105">
+        <v>619</v>
+      </c>
+      <c r="C105" t="s">
+        <v>5</v>
+      </c>
+      <c r="D105" t="s">
+        <v>25</v>
+      </c>
+      <c r="F105">
+        <v>1.49</v>
+      </c>
+      <c r="J105" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>15</v>
+      </c>
+      <c r="B106">
+        <v>647</v>
+      </c>
+      <c r="C106" t="s">
+        <v>5</v>
+      </c>
+      <c r="D106" t="s">
+        <v>40</v>
+      </c>
+      <c r="F106">
+        <v>0.3</v>
+      </c>
+      <c r="J106" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>15</v>
+      </c>
+      <c r="B107">
+        <v>647</v>
+      </c>
+      <c r="C107" t="s">
+        <v>5</v>
+      </c>
+      <c r="D107" t="s">
+        <v>23</v>
+      </c>
+      <c r="F107">
+        <v>0.38</v>
+      </c>
+      <c r="J107" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>15</v>
+      </c>
+      <c r="B108">
+        <v>647</v>
+      </c>
+      <c r="C108" t="s">
+        <v>5</v>
+      </c>
+      <c r="D108" t="s">
+        <v>21</v>
+      </c>
+      <c r="F108">
+        <v>0.34</v>
+      </c>
+      <c r="J108" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>15</v>
+      </c>
+      <c r="B109">
+        <v>647</v>
+      </c>
+      <c r="C109" t="s">
+        <v>5</v>
+      </c>
+      <c r="D109" t="s">
+        <v>24</v>
+      </c>
+      <c r="F109">
+        <v>0.43</v>
+      </c>
+      <c r="J109" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>15</v>
+      </c>
+      <c r="B110">
+        <v>647</v>
+      </c>
+      <c r="C110" t="s">
+        <v>5</v>
+      </c>
+      <c r="D110" t="s">
+        <v>25</v>
+      </c>
+      <c r="F110">
+        <v>0.35</v>
+      </c>
+      <c r="J110" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="113" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K113" s="1"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J62" xr:uid="{52DE5DE2-3EF6-48AC-A4A4-AF66BBBA5C59}"/>
+  <autoFilter ref="A1:J110" xr:uid="{52DE5DE2-3EF6-48AC-A4A4-AF66BBBA5C59}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="647"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Jupiter"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE353927-3316-47B7-93C4-1DC1B42CB65F}">
+  <dimension ref="A1:A28"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1">
+        <v>1.9797787919333132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>1.7146487641415433</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>2.0422536875760215</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>1.8736615817081201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>1.6475952181575622</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>1.9541259687134698</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>1.95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <f>AVERAGE(A1:A24)</f>
+        <v>1.6138360005095846</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <f>MAX(A1:A24)</f>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
+        <f>MIN(A1:A24)</f>
+        <v>0.91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Spectral Modeling and Trans vs EW Fit
NH3_Filter_Library_P3.py was updated as I addressed a paper question about the ratio of EW/Trans (or EW/Tau) from Pat Irwin.
</commit_message>
<xml_diff>
--- a/Literature CH4 and NH3 Measurements.xlsx
+++ b/Literature CH4 and NH3 Measurements.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Astronomy\Projects\SAS 2021 Ammonia\Jupiter_NH3_Analysis_P3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8659525D-C285-40FA-B939-A17396EA9F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586DEB97-FB2F-42B5-92C6-3366F0093368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DE140F0E-5E6A-4D54-8374-BA43FF538A80}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{DE140F0E-5E6A-4D54-8374-BA43FF538A80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$110</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="55">
   <si>
     <t>Molecule</t>
   </si>
@@ -236,12 +237,51 @@
   <si>
     <t>[Morena &amp; Molina, 1991]</t>
   </si>
+  <si>
+    <t>nm</t>
+  </si>
+  <si>
+    <t>cm-1</t>
+  </si>
+  <si>
+    <t>Meas EW</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>(cm-1/m-atm)</t>
+  </si>
+  <si>
+    <t>(nm/m-atm)</t>
+  </si>
+  <si>
+    <t>m-atm</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>dL</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,6 +297,21 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -284,12 +339,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,11 +664,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12:F110"/>
+      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3505,11 +3562,530 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50A79188-2C3C-4643-BD84-6BE6716CE7DE}">
+  <dimension ref="A1:M30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="I2">
+        <v>650</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+      <c r="K2">
+        <f>10000000/I2</f>
+        <v>15384.615384615385</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <f>(1-L2)*J2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>0.66</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3">
+        <v>650</v>
+      </c>
+      <c r="J3">
+        <v>10</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K12" si="0">10000000/I3</f>
+        <v>15384.615384615385</v>
+      </c>
+      <c r="L3">
+        <v>0.9</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M12" si="1">(1-L3)*J3</f>
+        <v>0.99999999999999978</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <f>0.5*B3+B15</f>
+        <v>647.33000000000004</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C5" si="2">10000000/B4</f>
+        <v>15448.071308297158</v>
+      </c>
+      <c r="I4">
+        <v>650</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>15384.615384615385</v>
+      </c>
+      <c r="L4">
+        <v>0.8</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="1"/>
+        <v>1.9999999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <f>B15-B3*0.5</f>
+        <v>646.66999999999996</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="2"/>
+        <v>15463.837815268995</v>
+      </c>
+      <c r="I5">
+        <v>650</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>15384.615384615385</v>
+      </c>
+      <c r="L5">
+        <v>0.7</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="1"/>
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <f>C5-C4</f>
+        <v>15.766506971836861</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6">
+        <v>650</v>
+      </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>15384.615384615385</v>
+      </c>
+      <c r="L6">
+        <v>0.6</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="I7">
+        <v>650</v>
+      </c>
+      <c r="J7">
+        <v>10</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>15384.615384615385</v>
+      </c>
+      <c r="L7">
+        <v>0.5</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8">
+        <v>650</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>15384.615384615385</v>
+      </c>
+      <c r="L8">
+        <v>0.4</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D9">
+        <f>C6/B3</f>
+        <v>23.888646927025547</v>
+      </c>
+      <c r="I9">
+        <v>650</v>
+      </c>
+      <c r="J9">
+        <v>10</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>15384.615384615385</v>
+      </c>
+      <c r="L9">
+        <v>0.3</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <v>550</v>
+      </c>
+      <c r="C10">
+        <f>10000000/B10</f>
+        <v>18181.81818181818</v>
+      </c>
+      <c r="F10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I10">
+        <v>650</v>
+      </c>
+      <c r="J10">
+        <v>10</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>15384.615384615385</v>
+      </c>
+      <c r="L10">
+        <v>0.2</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11">
+        <f>B13-B12</f>
+        <v>2.9039999999440624E-3</v>
+      </c>
+      <c r="C11" s="3">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="D11">
+        <f>C11/B11</f>
+        <v>33.057851240306192</v>
+      </c>
+      <c r="F11">
+        <v>15</v>
+      </c>
+      <c r="G11">
+        <f>F11*B11</f>
+        <v>4.3559999999160937E-2</v>
+      </c>
+      <c r="I11">
+        <v>650</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>15384.615384615385</v>
+      </c>
+      <c r="L11">
+        <v>0.1</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B12">
+        <f>10000000/C12</f>
+        <v>549.99854800383332</v>
+      </c>
+      <c r="C12">
+        <f>C$10+0.5*C11</f>
+        <v>18181.866181818179</v>
+      </c>
+      <c r="I12">
+        <v>650</v>
+      </c>
+      <c r="J12">
+        <v>10</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>15384.615384615385</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B13">
+        <f>10000000/C13</f>
+        <v>550.00145200383326</v>
+      </c>
+      <c r="C13">
+        <f>C$10-0.5*C11</f>
+        <v>18181.770181818181</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B15">
+        <v>647</v>
+      </c>
+      <c r="C15">
+        <f>10000000/B15</f>
+        <v>15455.950540958269</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17">
+        <f>B19-B18</f>
+        <v>2.6372367010935704E-2</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.63</v>
+      </c>
+      <c r="D17">
+        <f>C17/B17</f>
+        <v>23.888640702549033</v>
+      </c>
+      <c r="F17">
+        <v>15</v>
+      </c>
+      <c r="G17">
+        <f>F17*B17</f>
+        <v>0.39558550516403557</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B18">
+        <f>10000000/C18</f>
+        <v>646.98681408523555</v>
+      </c>
+      <c r="C18">
+        <f>C15+0.5*C17</f>
+        <v>15456.265540958269</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B19">
+        <f>10000000/C19</f>
+        <v>647.01318645224649</v>
+      </c>
+      <c r="C19">
+        <f>C15-0.5*C17</f>
+        <v>15455.635540958268</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="4">
+        <f>B24-B23</f>
+        <v>6.1955552208910376</v>
+      </c>
+      <c r="C22" s="3">
+        <v>148</v>
+      </c>
+      <c r="D22">
+        <f>C22/B22</f>
+        <v>23.888093112454708</v>
+      </c>
+      <c r="F22">
+        <v>300</v>
+      </c>
+      <c r="G22">
+        <f>F22*B22</f>
+        <v>1858.6665662673113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B23">
+        <f>10000000/C23</f>
+        <v>643.91705392919778</v>
+      </c>
+      <c r="C23">
+        <f>C15+0.5*C22</f>
+        <v>15529.950540958269</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B24">
+        <f>10000000/C24</f>
+        <v>650.11260915008882</v>
+      </c>
+      <c r="C24">
+        <f>C15-0.5*C22</f>
+        <v>15381.950540958269</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B26">
+        <v>619</v>
+      </c>
+      <c r="C26">
+        <f>10000000/B26</f>
+        <v>16155.088852988691</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" t="s">
+        <v>48</v>
+      </c>
+      <c r="F27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="4">
+        <f>B30-B29</f>
+        <v>4.7128803000759945E-3</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.123</v>
+      </c>
+      <c r="D28">
+        <f>C28/B28</f>
+        <v>26.098689584375109</v>
+      </c>
+      <c r="F28">
+        <v>300</v>
+      </c>
+      <c r="G28">
+        <f>F28*B28</f>
+        <v>1.4138640900227983</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B29">
+        <f>10000000/C29</f>
+        <v>618.99764356882065</v>
+      </c>
+      <c r="C29">
+        <f>C$26+0.5*C28</f>
+        <v>16155.15035298869</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B30">
+        <f>10000000/C30</f>
+        <v>619.00235644912073</v>
+      </c>
+      <c r="C30">
+        <f>C$26-0.5*C28</f>
+        <v>16155.027352988691</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE353927-3316-47B7-93C4-1DC1B42CB65F}">
   <dimension ref="A1:A28"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>